<commit_message>
finished calculating and writing roto stats
</commit_message>
<xml_diff>
--- a/src/main/resources/files/stats.xlsx
+++ b/src/main/resources/files/stats.xlsx
@@ -290,10 +290,10 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="A1:G1"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -675,10 +675,10 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K29" activeCellId="1" sqref="A1:G1 K29"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -708,7 +708,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>1401</v>
@@ -731,7 +731,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>1285</v>
@@ -754,7 +754,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>1184</v>
@@ -789,7 +789,7 @@
         <v>1.17</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>27</v>
@@ -915,7 +915,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>1309</v>
@@ -984,7 +984,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>1282</v>

</xml_diff>

<commit_message>
refactored for code cleanliness, saving before db addition
</commit_message>
<xml_diff>
--- a/src/main/resources/files/stats.xlsx
+++ b/src/main/resources/files/stats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -289,11 +289,11 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -349,7 +349,7 @@
         <v>643</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>665</v>
@@ -395,7 +395,7 @@
         <v>711</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>596</v>
@@ -404,7 +404,7 @@
         <v>44</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.242</v>
+        <v>0.252</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>0.754</v>
@@ -438,13 +438,13 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>623</v>
+        <v>603</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>183</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>647</v>
+        <v>607</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>89</v>
@@ -674,11 +674,11 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
cleaning up last flow
</commit_message>
<xml_diff>
--- a/src/main/resources/files/stats.xlsx
+++ b/src/main/resources/files/stats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -111,7 +111,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -149,13 +149,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -203,7 +196,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -213,10 +206,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -300,11 +289,11 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -334,22 +323,22 @@
         <v>7</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>682</v>
+        <v>722</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>118</v>
+        <v>168</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>644</v>
+        <v>684</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0.248</v>
+        <v>0.247</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>0.75</v>
+        <v>0.755</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -357,7 +346,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>182</v>
@@ -403,22 +392,22 @@
         <v>10</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>701</v>
+        <v>741</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>696</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.272</v>
+        <v>0.274</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>0.777</v>
+        <v>0.788</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -530,10 +519,10 @@
         <v>103</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0.259</v>
+        <v>0.26</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>0.771</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -563,8 +552,8 @@
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="3" t="n">
-        <v>660</v>
+      <c r="B12" s="2" t="n">
+        <v>688</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>192</v>
@@ -586,11 +575,11 @@
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="3" t="n">
-        <v>660</v>
+      <c r="B13" s="2" t="n">
+        <v>688</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>593</v>
@@ -632,7 +621,7 @@
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="2" t="n">
         <v>660</v>
       </c>
       <c r="C15" s="2" t="n">
@@ -685,11 +674,11 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -725,10 +714,10 @@
         <v>1606</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>3.95</v>
+        <v>3.9</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>1.22</v>
+        <v>1.2</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>108</v>
@@ -817,10 +806,10 @@
         <v>1559</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>4.55</v>
+        <v>4.65</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>1.17</v>
+        <v>1.18</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>124</v>
@@ -863,10 +852,10 @@
         <v>1503</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>3.51</v>
+        <v>3.48</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>1.16</v>
+        <v>1.11</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>103</v>

</xml_diff>

<commit_message>
moved to strategy with values added via property file for spring beans and is working
</commit_message>
<xml_diff>
--- a/src/main/resources/files/stats.xlsx
+++ b/src/main/resources/files/stats.xlsx
@@ -5,11 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="CHAMPIONS Hitting" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="CHAMPIONS Pitching" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="27">
   <si>
     <t xml:space="preserve">N</t>
   </si>
@@ -289,11 +291,11 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -674,11 +676,11 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1050,4 +1052,774 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>722</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>168</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>684</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>95</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>0.247</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>0.755</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>644</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>182</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>665</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>66</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>0.245</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>0.733</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>682</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>192</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>637</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>0.241</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>0.732</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>641</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>207</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>696</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>0.274</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>0.788</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>701</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>184</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>663</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>99</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>0.253</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>603</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>183</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>607</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>89</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0.263</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>0.785</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>632</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>183</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>659</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>0.744</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>658</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>179</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>679</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>0.259</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>0.757</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>682</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>177</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>643</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>103</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>618</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>174</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>638</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>0.257</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>0.763</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>688</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>192</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>617</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>93</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>0.254</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>0.757</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>688</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>169</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>593</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>0.268</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>0.786</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>660</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>155</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>621</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>0.257</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>0.741</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>660</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>142</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>571</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>108</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>0.269</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>0.748</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="GOD WILLS IT"/>
+    <hyperlink ref="A3" r:id="rId2" display="Mac"/>
+    <hyperlink ref="A4" r:id="rId3" display="Epic7"/>
+    <hyperlink ref="A5" r:id="rId4" display="rainmaker"/>
+    <hyperlink ref="A6" r:id="rId5" display="EL Onće"/>
+    <hyperlink ref="A7" r:id="rId6" display="confusion"/>
+    <hyperlink ref="A8" r:id="rId7" display="Swampnuts"/>
+    <hyperlink ref="A9" r:id="rId8" display="Samsquanches"/>
+    <hyperlink ref="A10" r:id="rId9" display="Lundo’s Legends"/>
+    <hyperlink ref="A11" r:id="rId10" display="SmokeWalkers"/>
+    <hyperlink ref="A12" r:id="rId11" display="MillerTime"/>
+    <hyperlink ref="A13" r:id="rId12" display="DJ's Quality Team"/>
+    <hyperlink ref="A14" r:id="rId13" display="Splitfinger Skadoosh"/>
+    <hyperlink ref="A15" r:id="rId14" display="Corbin Copy"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>97</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>1606</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>108</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>96</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>1386</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>4.67</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>104</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>91</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>1285</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>96</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>1427</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>109</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>115</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>1559</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>4.65</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>124</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>87</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1375</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>107</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>1503</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>3.48</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>103</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>104</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>122</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>1299</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>106</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1507</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>3.55</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>95</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>92</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>1566</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>119</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>109</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>1556</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>136</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>103</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>1359</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>3.91</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>98</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>1308</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>89</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="GOD WILLS IT"/>
+    <hyperlink ref="A3" r:id="rId2" display="confusion"/>
+    <hyperlink ref="A4" r:id="rId3" display="DJ's Quality Team"/>
+    <hyperlink ref="A5" r:id="rId4" display="Epic7"/>
+    <hyperlink ref="A6" r:id="rId5" display="Lundo’s Legends"/>
+    <hyperlink ref="A7" r:id="rId6" display="MillerTime"/>
+    <hyperlink ref="A8" r:id="rId7" display="rainmaker"/>
+    <hyperlink ref="A9" r:id="rId8" display="Samsquanches"/>
+    <hyperlink ref="A10" r:id="rId9" display="SmokeWalkers"/>
+    <hyperlink ref="A11" r:id="rId10" display="Splitfinger Skadoosh"/>
+    <hyperlink ref="A12" r:id="rId11" display="Swampnuts"/>
+    <hyperlink ref="A13" r:id="rId12" display="EL Onće"/>
+    <hyperlink ref="A14" r:id="rId13" display="Mac"/>
+    <hyperlink ref="A15" r:id="rId14" display="Corbin Copy"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
separated RankService into new class from RotoS
</commit_message>
<xml_diff>
--- a/src/main/resources/files/stats.xlsx
+++ b/src/main/resources/files/stats.xlsx
@@ -295,7 +295,7 @@
       <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -680,7 +680,7 @@
       <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1062,10 +1062,10 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1371,7 +1371,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>155</v>
@@ -1450,7 +1450,7 @@
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
working on 2nd league, need to add 2nd set of pojo's
</commit_message>
<xml_diff>
--- a/src/main/resources/files/stats.xlsx
+++ b/src/main/resources/files/stats.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="PSD Hitting" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="PSD Pitching" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="CHAMPIONS Hitting" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="CHAMPIONS Pitching" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="27">
   <si>
     <t xml:space="preserve">N</t>
   </si>
@@ -40,70 +40,70 @@
     <t xml:space="preserve">SB</t>
   </si>
   <si>
+    <t xml:space="preserve">OPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOD WILLS IT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confusion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epic7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rainmaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samsquanches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lundo’s Legends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SmokeWalkers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MillerTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DJ's Quality Team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Splitfinger Skadoosh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSV</t>
+  </si>
+  <si>
     <t xml:space="preserve">AVG</t>
   </si>
   <si>
-    <t xml:space="preserve">OPS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GOD WILLS IT</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mac</t>
   </si>
   <si>
-    <t xml:space="preserve">Epic7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rainmaker</t>
-  </si>
-  <si>
     <t xml:space="preserve">EL Onće</t>
   </si>
   <si>
-    <t xml:space="preserve">confusion</t>
-  </si>
-  <si>
     <t xml:space="preserve">Swampnuts</t>
   </si>
   <si>
-    <t xml:space="preserve">Samsquanches</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lundo’s Legends</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SmokeWalkers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MillerTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DJ's Quality Team</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Splitfinger Skadoosh</t>
-  </si>
-  <si>
     <t xml:space="preserve">Corbin Copy</t>
   </si>
   <si>
     <t xml:space="preserve">W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WHIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSV</t>
   </si>
 </sst>
 </file>
@@ -289,13 +289,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -316,13 +316,10 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>722</v>
@@ -337,38 +334,32 @@
         <v>95</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0.247</v>
-      </c>
-      <c r="G2" s="2" t="n">
         <v>0.755</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>644</v>
+        <v>603</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>665</v>
+        <v>607</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0.245</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>0.733</v>
+        <v>0.785</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>682</v>
@@ -383,15 +374,12 @@
         <v>65</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0.241</v>
-      </c>
-      <c r="G4" s="2" t="n">
         <v>0.732</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>741</v>
@@ -406,258 +394,141 @@
         <v>148</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.274</v>
-      </c>
-      <c r="G5" s="2" t="n">
         <v>0.788</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>701</v>
+        <v>658</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>663</v>
+        <v>679</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0.253</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>0.75</v>
+        <v>0.757</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>603</v>
+        <v>682</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>607</v>
+        <v>643</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>0.263</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>0.785</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>632</v>
+        <v>618</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>659</v>
+        <v>638</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="G8" s="2" t="n">
-        <v>0.744</v>
+        <v>0.763</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>658</v>
+        <v>688</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>679</v>
+        <v>617</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>0.259</v>
-      </c>
-      <c r="G9" s="2" t="n">
         <v>0.757</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>682</v>
+        <v>688</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>643</v>
+        <v>593</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>103</v>
+        <v>41</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0.26</v>
-      </c>
-      <c r="G10" s="2" t="n">
-        <v>0.77</v>
+        <v>0.786</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>618</v>
+        <v>660</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>638</v>
+        <v>621</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0.257</v>
-      </c>
-      <c r="G11" s="2" t="n">
-        <v>0.763</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>688</v>
-      </c>
-      <c r="C12" s="2" t="n">
-        <v>192</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>617</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>93</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <v>0.254</v>
-      </c>
-      <c r="G12" s="2" t="n">
-        <v>0.757</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="2" t="n">
-        <v>688</v>
-      </c>
-      <c r="C13" s="2" t="n">
-        <v>169</v>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>593</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="F13" s="2" t="n">
-        <v>0.268</v>
-      </c>
-      <c r="G13" s="2" t="n">
-        <v>0.786</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>660</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>155</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>621</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>72</v>
-      </c>
-      <c r="F14" s="2" t="n">
-        <v>0.257</v>
-      </c>
-      <c r="G14" s="2" t="n">
         <v>0.741</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>660</v>
-      </c>
-      <c r="C15" s="2" t="n">
-        <v>142</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>571</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>108</v>
-      </c>
-      <c r="F15" s="2" t="n">
-        <v>0.268</v>
-      </c>
-      <c r="G15" s="2" t="n">
-        <v>0.748</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="GOD WILLS IT"/>
-    <hyperlink ref="A3" r:id="rId2" display="Mac"/>
+    <hyperlink ref="A3" r:id="rId2" display="confusion"/>
     <hyperlink ref="A4" r:id="rId3" display="Epic7"/>
     <hyperlink ref="A5" r:id="rId4" display="rainmaker"/>
-    <hyperlink ref="A6" r:id="rId5" display="EL Onće"/>
-    <hyperlink ref="A7" r:id="rId6" display="confusion"/>
-    <hyperlink ref="A8" r:id="rId7" display="Swampnuts"/>
-    <hyperlink ref="A9" r:id="rId8" display="Samsquanches"/>
-    <hyperlink ref="A10" r:id="rId9" display="Lundo’s Legends"/>
-    <hyperlink ref="A11" r:id="rId10" display="SmokeWalkers"/>
-    <hyperlink ref="A12" r:id="rId11" display="MillerTime"/>
-    <hyperlink ref="A13" r:id="rId12" display="DJ's Quality Team"/>
-    <hyperlink ref="A14" r:id="rId13" display="Splitfinger Skadoosh"/>
-    <hyperlink ref="A15" r:id="rId14" display="Corbin Copy"/>
+    <hyperlink ref="A6" r:id="rId5" display="Samsquanches"/>
+    <hyperlink ref="A7" r:id="rId6" display="Lundo’s Legends"/>
+    <hyperlink ref="A8" r:id="rId7" display="SmokeWalkers"/>
+    <hyperlink ref="A9" r:id="rId8" display="MillerTime"/>
+    <hyperlink ref="A10" r:id="rId9" display="DJ's Quality Team"/>
+    <hyperlink ref="A11" r:id="rId10" display="Splitfinger Skadoosh"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -674,359 +545,268 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>97</v>
+        <v>1606</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>1606</v>
+        <v>3.9</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>3.9</v>
+        <v>1.2</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>1.2</v>
+        <v>108</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>108</v>
-      </c>
-      <c r="G2" s="2" t="n">
         <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>96</v>
+        <v>1386</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>1386</v>
+        <v>4.67</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>4.67</v>
+        <v>1.37</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>1.37</v>
+        <v>104</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>104</v>
-      </c>
-      <c r="G3" s="2" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>91</v>
+        <v>1285</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>1285</v>
+        <v>2.04</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>2.04</v>
+        <v>1.23</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>1.23</v>
+        <v>100</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="G4" s="2" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>96</v>
+        <v>1427</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>1427</v>
+        <v>3.78</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>3.78</v>
+        <v>1.19</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>1.19</v>
+        <v>109</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>109</v>
-      </c>
-      <c r="G5" s="2" t="n">
         <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>115</v>
+        <v>1559</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>1559</v>
+        <v>4.65</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>4.65</v>
+        <v>1.18</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>1.18</v>
+        <v>124</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>124</v>
-      </c>
-      <c r="G6" s="2" t="n">
         <v>49</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>87</v>
+        <v>1375</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>1375</v>
+        <v>3.84</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>3.84</v>
+        <v>1.14</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>1.14</v>
+        <v>107</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>107</v>
-      </c>
-      <c r="G7" s="2" t="n">
         <v>36</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>90</v>
+        <v>1503</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>1503</v>
+        <v>3.48</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>3.48</v>
+        <v>1.11</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>1.11</v>
+        <v>103</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>103</v>
-      </c>
-      <c r="G8" s="2" t="n">
         <v>81</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>104</v>
+        <v>1500</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>1500</v>
+        <v>3.72</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>3.72</v>
+        <v>1.34</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>1.34</v>
+        <v>122</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>122</v>
-      </c>
-      <c r="G9" s="2" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2" t="n">
+        <v>1299</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="E10" s="2" t="n">
         <v>74</v>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>1299</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>3.71</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>1.21</v>
-      </c>
       <c r="F10" s="2" t="n">
-        <v>74</v>
-      </c>
-      <c r="G10" s="2" t="n">
         <v>95</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>96</v>
+        <v>1507</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>1507</v>
+        <v>3.55</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>3.55</v>
+        <v>1.28</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>1.28</v>
+        <v>95</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>95</v>
-      </c>
-      <c r="G11" s="2" t="n">
         <v>65</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>92</v>
-      </c>
-      <c r="C12" s="2" t="n">
-        <v>1566</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>3.81</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <v>119</v>
-      </c>
-      <c r="G12" s="2" t="n">
-        <v>39</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="n">
-        <v>109</v>
-      </c>
-      <c r="C13" s="2" t="n">
-        <v>1556</v>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>3.42</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>1.36</v>
-      </c>
-      <c r="F13" s="2" t="n">
-        <v>136</v>
-      </c>
-      <c r="G13" s="2" t="n">
-        <v>8</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>103</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>1359</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>3.91</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="F14" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="G14" s="2" t="n">
-        <v>31</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>98</v>
-      </c>
-      <c r="C15" s="2" t="n">
-        <v>1308</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>4.16</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>1.21</v>
-      </c>
-      <c r="F15" s="2" t="n">
-        <v>89</v>
-      </c>
-      <c r="G15" s="2" t="n">
-        <v>31</v>
-      </c>
-    </row>
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="GOD WILLS IT"/>
@@ -1039,10 +819,6 @@
     <hyperlink ref="A9" r:id="rId8" display="Samsquanches"/>
     <hyperlink ref="A10" r:id="rId9" display="SmokeWalkers"/>
     <hyperlink ref="A11" r:id="rId10" display="Splitfinger Skadoosh"/>
-    <hyperlink ref="A12" r:id="rId11" display="Swampnuts"/>
-    <hyperlink ref="A13" r:id="rId12" display="EL Onće"/>
-    <hyperlink ref="A14" r:id="rId13" display="Mac"/>
-    <hyperlink ref="A15" r:id="rId14" display="Corbin Copy"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1061,11 +837,11 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1084,15 +860,15 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>722</v>
@@ -1115,7 +891,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>644</v>
@@ -1138,7 +914,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>682</v>
@@ -1161,7 +937,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>641</v>
@@ -1184,7 +960,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>701</v>
@@ -1207,7 +983,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>603</v>
@@ -1230,7 +1006,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>632</v>
@@ -1253,7 +1029,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>658</v>
@@ -1276,7 +1052,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>682</v>
@@ -1299,7 +1075,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>618</v>
@@ -1322,7 +1098,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>688</v>
@@ -1345,7 +1121,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>688</v>
@@ -1368,7 +1144,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>661</v>
@@ -1391,7 +1167,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>660</v>
@@ -1450,34 +1226,34 @@
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>97</v>
@@ -1500,7 +1276,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>96</v>
@@ -1523,7 +1299,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>91</v>
@@ -1546,7 +1322,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>96</v>
@@ -1569,7 +1345,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>115</v>
@@ -1592,7 +1368,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>87</v>
@@ -1615,7 +1391,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>90</v>
@@ -1638,7 +1414,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>104</v>
@@ -1661,7 +1437,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>74</v>
@@ -1684,7 +1460,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>106</v>
@@ -1707,7 +1483,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>92</v>
@@ -1730,7 +1506,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>109</v>
@@ -1753,7 +1529,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>103</v>
@@ -1776,7 +1552,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>98</v>

</xml_diff>

<commit_message>
fixed bugs related to using two leagues and set up runner so that all modifications can be done in property file
</commit_message>
<xml_diff>
--- a/src/main/resources/files/stats.xlsx
+++ b/src/main/resources/files/stats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PSD Hitting" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="27">
   <si>
     <t xml:space="preserve">N</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">OPS</t>
   </si>
   <si>
+    <t xml:space="preserve">AVG</t>
+  </si>
+  <si>
     <t xml:space="preserve">GOD WILLS IT</t>
   </si>
   <si>
@@ -88,7 +91,7 @@
     <t xml:space="preserve">NSV</t>
   </si>
   <si>
-    <t xml:space="preserve">AVG</t>
+    <t xml:space="preserve">W</t>
   </si>
   <si>
     <t xml:space="preserve">Mac</t>
@@ -101,9 +104,6 @@
   </si>
   <si>
     <t xml:space="preserve">Corbin Copy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W</t>
   </si>
 </sst>
 </file>
@@ -289,13 +289,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -316,10 +316,13 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>722</v>
@@ -339,7 +342,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>603</v>
@@ -359,7 +362,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>682</v>
@@ -379,7 +382,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>741</v>
@@ -399,7 +402,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>658</v>
@@ -419,7 +422,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>682</v>
@@ -439,7 +442,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>618</v>
@@ -459,7 +462,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>688</v>
@@ -479,7 +482,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>688</v>
@@ -499,7 +502,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>660</v>
@@ -545,37 +548,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>1606</v>
@@ -595,7 +601,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>1386</v>
@@ -615,7 +621,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>1285</v>
@@ -635,7 +641,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>1427</v>
@@ -655,7 +661,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>1559</v>
@@ -675,7 +681,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>1375</v>
@@ -695,7 +701,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>1503</v>
@@ -715,7 +721,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>1500</v>
@@ -735,7 +741,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>1299</v>
@@ -755,7 +761,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>1507</v>
@@ -841,7 +847,7 @@
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -860,7 +866,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>5</v>
@@ -868,7 +874,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>722</v>
@@ -891,7 +897,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>644</v>
@@ -914,7 +920,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>682</v>
@@ -937,7 +943,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>641</v>
@@ -960,7 +966,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>701</v>
@@ -983,7 +989,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>603</v>
@@ -1006,7 +1012,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>632</v>
@@ -1029,7 +1035,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>658</v>
@@ -1052,7 +1058,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>682</v>
@@ -1075,7 +1081,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>618</v>
@@ -1098,7 +1104,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>688</v>
@@ -1121,7 +1127,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>688</v>
@@ -1144,7 +1150,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>661</v>
@@ -1167,7 +1173,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>660</v>
@@ -1226,34 +1232,34 @@
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>97</v>
@@ -1276,7 +1282,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>96</v>
@@ -1299,7 +1305,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>91</v>
@@ -1322,7 +1328,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>96</v>
@@ -1345,7 +1351,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>115</v>
@@ -1368,7 +1374,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>87</v>
@@ -1391,7 +1397,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>90</v>
@@ -1414,7 +1420,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>104</v>
@@ -1437,7 +1443,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>74</v>
@@ -1460,7 +1466,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>106</v>
@@ -1483,7 +1489,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>92</v>
@@ -1506,7 +1512,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>109</v>
@@ -1529,7 +1535,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>103</v>
@@ -1552,7 +1558,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>98</v>

</xml_diff>

<commit_message>
in progress work on changing league
</commit_message>
<xml_diff>
--- a/src/main/resources/files/stats.xlsx
+++ b/src/main/resources/files/stats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="PSD Hitting" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,8 @@
     <sheet name="CHAMPIONS Hitting" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="CHAMPIONS Pitching" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="CHAMPIONS" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="PSD" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Standard" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="41">
   <si>
     <t xml:space="preserve">N</t>
   </si>
@@ -108,6 +110,45 @@
   </si>
   <si>
     <t xml:space="preserve">Team Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walks and Balks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jags In 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slobber Knockers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reno Giants 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feeling Ucey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Black Hole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apple Pie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">𝙍 𝙊 𝘾 𝙆 ®</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IALO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steel Wheels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kansas City BBQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ever Dream</t>
   </si>
 </sst>
 </file>
@@ -316,10 +357,10 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.25390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -575,10 +616,10 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.25390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -871,7 +912,7 @@
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1256,7 +1297,7 @@
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1637,11 +1678,11 @@
   </sheetPr>
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H35" activeCellId="0" sqref="H35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -2354,4 +2395,1022 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>722</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>168</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>684</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>95</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>0.755</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>1606</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>108</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>603</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>183</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>607</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>89</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>1386</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>4.67</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>104</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>682</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>192</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>637</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>0.732</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>1285</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>741</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>207</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>696</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>148</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>0.788</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>1427</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>109</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>658</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>179</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>679</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>77</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>0.757</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>1559</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>4.65</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>124</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>682</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>177</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>643</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>103</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>1375</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>107</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>618</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>174</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>638</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>0.763</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>1503</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>3.48</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>103</v>
+      </c>
+      <c r="L8" s="2" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>688</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>192</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>617</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>93</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>0.757</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>1500</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>122</v>
+      </c>
+      <c r="L9" s="2" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>688</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>169</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>593</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>0.786</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>1299</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="L10" s="2" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>660</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>155</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>621</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>0.741</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>1507</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>3.55</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>95</v>
+      </c>
+      <c r="L11" s="2" t="n">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="GOD WILLS IT"/>
+    <hyperlink ref="G2" r:id="rId2" display="GOD WILLS IT"/>
+    <hyperlink ref="A3" r:id="rId3" display="confusion"/>
+    <hyperlink ref="G3" r:id="rId4" display="confusion"/>
+    <hyperlink ref="A4" r:id="rId5" display="Epic7"/>
+    <hyperlink ref="G4" r:id="rId6" display="Epic7"/>
+    <hyperlink ref="A5" r:id="rId7" display="rainmaker"/>
+    <hyperlink ref="G5" r:id="rId8" display="rainmaker"/>
+    <hyperlink ref="A6" r:id="rId9" display="Samsquanches"/>
+    <hyperlink ref="G6" r:id="rId10" display="Samsquanches"/>
+    <hyperlink ref="A7" r:id="rId11" display="Lundo’s Legends"/>
+    <hyperlink ref="G7" r:id="rId12" display="Lundo’s Legends"/>
+    <hyperlink ref="A8" r:id="rId13" display="SmokeWalkers"/>
+    <hyperlink ref="G8" r:id="rId14" display="SmokeWalkers"/>
+    <hyperlink ref="A9" r:id="rId15" display="MillerTime"/>
+    <hyperlink ref="G9" r:id="rId16" display="MillerTime"/>
+    <hyperlink ref="A10" r:id="rId17" display="DJ's Quality Team"/>
+    <hyperlink ref="G10" r:id="rId18" display="DJ's Quality Team"/>
+    <hyperlink ref="A11" r:id="rId19" display="Splitfinger Skadoosh"/>
+    <hyperlink ref="G11" r:id="rId20" display="Splitfinger Skadoosh"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K26" activeCellId="0" sqref="K26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="K2" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="L2" s="5" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="L3" s="5" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="L4" s="5" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="K5" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="L5" s="5" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="L6" s="5" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="L7" s="5" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="K8" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="L8" s="5" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="L9" s="5" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="L10" s="5" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="L11" s="5" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="L12" s="5" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="5" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="L13" s="5" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" display="R"/>
+    <hyperlink ref="C1" r:id="rId2" display="HR"/>
+    <hyperlink ref="D1" r:id="rId3" display="RBI"/>
+    <hyperlink ref="E1" r:id="rId4" display="SB"/>
+    <hyperlink ref="F1" r:id="rId5" display="AVG"/>
+    <hyperlink ref="H1" r:id="rId6" display="W"/>
+    <hyperlink ref="I1" r:id="rId7" display="SV"/>
+    <hyperlink ref="J1" r:id="rId8" display="K"/>
+    <hyperlink ref="K1" r:id="rId9" display="ERA"/>
+    <hyperlink ref="L1" r:id="rId10" display="WHIP"/>
+    <hyperlink ref="A2" r:id="rId11" display="Walks and Balks"/>
+    <hyperlink ref="G2" r:id="rId12" display="Walks and Balks"/>
+    <hyperlink ref="A3" r:id="rId13" display="Jags In 2023"/>
+    <hyperlink ref="G3" r:id="rId14" display="Jags In 2023"/>
+    <hyperlink ref="A4" r:id="rId15" display="Slobber Knockers"/>
+    <hyperlink ref="G4" r:id="rId16" display="Slobber Knockers"/>
+    <hyperlink ref="A5" r:id="rId17" display="Reno Giants 2"/>
+    <hyperlink ref="G5" r:id="rId18" display="Reno Giants 2"/>
+    <hyperlink ref="A6" r:id="rId19" display="Feeling Ucey"/>
+    <hyperlink ref="G6" r:id="rId20" display="Feeling Ucey"/>
+    <hyperlink ref="A7" r:id="rId21" display="The Black Hole"/>
+    <hyperlink ref="G7" r:id="rId22" display="The Black Hole"/>
+    <hyperlink ref="A8" r:id="rId23" display="Apple Pie"/>
+    <hyperlink ref="G8" r:id="rId24" display="Apple Pie"/>
+    <hyperlink ref="A9" r:id="rId25" display="𝙍 𝙊 𝘾 𝙆 ®"/>
+    <hyperlink ref="G9" r:id="rId26" display="𝙍 𝙊 𝘾 𝙆 ®"/>
+    <hyperlink ref="A10" r:id="rId27" display="IALO"/>
+    <hyperlink ref="G10" r:id="rId28" display="IALO"/>
+    <hyperlink ref="A11" r:id="rId29" display="Steel Wheels"/>
+    <hyperlink ref="G11" r:id="rId30" display="Steel Wheels"/>
+    <hyperlink ref="A12" r:id="rId31" display="Kansas City BBQ"/>
+    <hyperlink ref="G12" r:id="rId32" display="Kansas City BBQ"/>
+    <hyperlink ref="A13" r:id="rId33" display="Ever Dream"/>
+    <hyperlink ref="G13" r:id="rId34" display="Ever Dream"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
completed logic to run regular roto for all leagues
</commit_message>
<xml_diff>
--- a/src/main/resources/files/stats.xlsx
+++ b/src/main/resources/files/stats.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="50">
   <si>
     <t xml:space="preserve">N</t>
   </si>
@@ -110,6 +110,33 @@
   </si>
   <si>
     <t xml:space="preserve">Team Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yeah Jeets!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raincrafter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cue the Duckboats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smokescreen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ShohTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RobbNen#31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leandres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joe's Nice Team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matt's Marvelous Team</t>
   </si>
   <si>
     <t xml:space="preserve">SV</t>
@@ -251,7 +278,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -274,6 +301,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -360,7 +391,7 @@
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.25390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.28125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -619,7 +650,7 @@
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.25390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.28125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -912,7 +943,7 @@
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1297,7 +1328,7 @@
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1682,7 +1713,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -2405,10 +2436,10 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -2449,407 +2480,407 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="E2" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>722</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>168</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>684</v>
-      </c>
-      <c r="E2" s="2" t="n">
+      <c r="F2" s="2" t="n">
+        <v>0.828</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>87</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>2.74</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>52</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>0.819</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>136</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>81</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>0.906</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>106</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>74</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>0.743</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>93</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>62</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>142</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>4.84</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>105</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="J8" s="2" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="L8" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>66</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>0.828</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>5.02</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="L9" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>0.723</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>109</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>5.15</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="L10" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>0.787</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="2" t="n">
         <v>95</v>
       </c>
-      <c r="F2" s="2" t="n">
-        <v>0.755</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>1606</v>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>3.9</v>
-      </c>
-      <c r="J2" s="2" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>108</v>
-      </c>
-      <c r="L2" s="2" t="n">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="I11" s="2" t="n">
+        <v>3.98</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="K11" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>603</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>183</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>607</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>89</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>0.785</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>1386</v>
-      </c>
-      <c r="I3" s="2" t="n">
-        <v>4.67</v>
-      </c>
-      <c r="J3" s="2" t="n">
-        <v>1.37</v>
-      </c>
-      <c r="K3" s="2" t="n">
-        <v>104</v>
-      </c>
-      <c r="L3" s="2" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>682</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>192</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>637</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>65</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>0.732</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>1285</v>
-      </c>
-      <c r="I4" s="2" t="n">
-        <v>2.04</v>
-      </c>
-      <c r="J4" s="2" t="n">
-        <v>1.23</v>
-      </c>
-      <c r="K4" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="L4" s="2" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>741</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>207</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>696</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>148</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>0.788</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="2" t="n">
-        <v>1427</v>
-      </c>
-      <c r="I5" s="2" t="n">
-        <v>3.78</v>
-      </c>
-      <c r="J5" s="2" t="n">
-        <v>1.19</v>
-      </c>
-      <c r="K5" s="2" t="n">
-        <v>109</v>
-      </c>
-      <c r="L5" s="2" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>658</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>179</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>679</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>77</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>0.757</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>1559</v>
-      </c>
-      <c r="I6" s="2" t="n">
-        <v>4.65</v>
-      </c>
-      <c r="J6" s="2" t="n">
-        <v>1.18</v>
-      </c>
-      <c r="K6" s="2" t="n">
-        <v>124</v>
-      </c>
-      <c r="L6" s="2" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>682</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>177</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>643</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>103</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>1375</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <v>3.84</v>
-      </c>
-      <c r="J7" s="2" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="K7" s="2" t="n">
-        <v>107</v>
-      </c>
-      <c r="L7" s="2" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2" t="n">
-        <v>618</v>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>174</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>638</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>55</v>
-      </c>
-      <c r="F8" s="2" t="n">
-        <v>0.763</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="2" t="n">
-        <v>1503</v>
-      </c>
-      <c r="I8" s="2" t="n">
-        <v>3.48</v>
-      </c>
-      <c r="J8" s="2" t="n">
-        <v>1.11</v>
-      </c>
-      <c r="K8" s="2" t="n">
-        <v>103</v>
-      </c>
-      <c r="L8" s="2" t="n">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>688</v>
-      </c>
-      <c r="C9" s="2" t="n">
-        <v>192</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>617</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>93</v>
-      </c>
-      <c r="F9" s="2" t="n">
-        <v>0.757</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="2" t="n">
-        <v>1500</v>
-      </c>
-      <c r="I9" s="2" t="n">
-        <v>3.72</v>
-      </c>
-      <c r="J9" s="2" t="n">
-        <v>1.34</v>
-      </c>
-      <c r="K9" s="2" t="n">
-        <v>122</v>
-      </c>
-      <c r="L9" s="2" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>688</v>
-      </c>
-      <c r="C10" s="2" t="n">
-        <v>169</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>593</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>0.786</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>1299</v>
-      </c>
-      <c r="I10" s="2" t="n">
-        <v>3.71</v>
-      </c>
-      <c r="J10" s="2" t="n">
-        <v>1.21</v>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>74</v>
-      </c>
-      <c r="L10" s="2" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>660</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>155</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>621</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>72</v>
-      </c>
-      <c r="F11" s="2" t="n">
-        <v>0.741</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>1507</v>
-      </c>
-      <c r="I11" s="2" t="n">
-        <v>3.55</v>
-      </c>
-      <c r="J11" s="2" t="n">
-        <v>1.28</v>
-      </c>
-      <c r="K11" s="2" t="n">
-        <v>95</v>
-      </c>
       <c r="L11" s="2" t="n">
-        <v>65</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="GOD WILLS IT"/>
-    <hyperlink ref="G2" r:id="rId2" display="GOD WILLS IT"/>
-    <hyperlink ref="A3" r:id="rId3" display="confusion"/>
-    <hyperlink ref="G3" r:id="rId4" display="confusion"/>
-    <hyperlink ref="A4" r:id="rId5" display="Epic7"/>
-    <hyperlink ref="G4" r:id="rId6" display="Epic7"/>
-    <hyperlink ref="A5" r:id="rId7" display="rainmaker"/>
-    <hyperlink ref="G5" r:id="rId8" display="rainmaker"/>
-    <hyperlink ref="A6" r:id="rId9" display="Samsquanches"/>
-    <hyperlink ref="G6" r:id="rId10" display="Samsquanches"/>
-    <hyperlink ref="A7" r:id="rId11" display="Lundo’s Legends"/>
-    <hyperlink ref="G7" r:id="rId12" display="Lundo’s Legends"/>
-    <hyperlink ref="A8" r:id="rId13" display="SmokeWalkers"/>
-    <hyperlink ref="G8" r:id="rId14" display="SmokeWalkers"/>
-    <hyperlink ref="A9" r:id="rId15" display="MillerTime"/>
-    <hyperlink ref="G9" r:id="rId16" display="MillerTime"/>
-    <hyperlink ref="A10" r:id="rId17" display="DJ's Quality Team"/>
-    <hyperlink ref="G10" r:id="rId18" display="DJ's Quality Team"/>
-    <hyperlink ref="A11" r:id="rId19" display="Splitfinger Skadoosh"/>
-    <hyperlink ref="G11" r:id="rId20" display="Splitfinger Skadoosh"/>
+    <hyperlink ref="A2" r:id="rId1" display="Yeah Jeets!"/>
+    <hyperlink ref="G2" r:id="rId2" display="Yeah Jeets!"/>
+    <hyperlink ref="A3" r:id="rId3" display="raincrafter"/>
+    <hyperlink ref="G3" r:id="rId4" display="raincrafter"/>
+    <hyperlink ref="A4" r:id="rId5" display="Cue the Duckboats"/>
+    <hyperlink ref="G4" r:id="rId6" display="Cue the Duckboats"/>
+    <hyperlink ref="A5" r:id="rId7" display="Smokescreen"/>
+    <hyperlink ref="G5" r:id="rId8" display="Smokescreen"/>
+    <hyperlink ref="A6" r:id="rId9" display="ShohTime"/>
+    <hyperlink ref="G6" r:id="rId10" display="ShohTime"/>
+    <hyperlink ref="A7" r:id="rId11" display="RobbNen#31"/>
+    <hyperlink ref="G7" r:id="rId12" display="RobbNen#31"/>
+    <hyperlink ref="A8" r:id="rId13" display="Epic7"/>
+    <hyperlink ref="G8" r:id="rId14" display="Epic7"/>
+    <hyperlink ref="A9" r:id="rId15" display="Leandres"/>
+    <hyperlink ref="G9" r:id="rId16" display="Leandres"/>
+    <hyperlink ref="A10" r:id="rId17" display="Joe's Nice Team"/>
+    <hyperlink ref="G10" r:id="rId18" display="Joe's Nice Team"/>
+    <hyperlink ref="A11" r:id="rId19" display="Matt's Marvelous Team"/>
+    <hyperlink ref="G11" r:id="rId20" display="Matt's Marvelous Team"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2869,10 +2900,10 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K26" activeCellId="0" sqref="K26"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -2900,7 +2931,7 @@
         <v>22</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>17</v>
@@ -2914,458 +2945,458 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B2" s="5" t="n">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="C2" s="5" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F2" s="5" t="n">
-        <v>0.11</v>
+        <v>0.305</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H2" s="5" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I2" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J2" s="5" t="n">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="K2" s="5" t="n">
-        <v>0.11</v>
+        <v>4.07</v>
       </c>
       <c r="L2" s="5" t="n">
-        <v>0.11</v>
+        <v>1.47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="C3" s="5" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.11</v>
+        <v>0.288</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="H3" s="5" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I3" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="5" t="n">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="K3" s="5" t="n">
-        <v>0.11</v>
+        <v>4.52</v>
       </c>
       <c r="L3" s="5" t="n">
-        <v>0.11</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.11</v>
+        <v>0.294</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="H4" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I4" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="5" t="n">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="K4" s="5" t="n">
-        <v>0.11</v>
+        <v>3.96</v>
       </c>
       <c r="L4" s="5" t="n">
-        <v>0.11</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>0.11</v>
+        <v>0.241</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="H5" s="5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I5" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J5" s="5" t="n">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="K5" s="5" t="n">
-        <v>0.11</v>
+        <v>4.55</v>
       </c>
       <c r="L5" s="5" t="n">
-        <v>0.11</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>0.11</v>
+        <v>0.271</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I6" s="5" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J6" s="5" t="n">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="K6" s="5" t="n">
-        <v>0.11</v>
+        <v>3.13</v>
       </c>
       <c r="L6" s="5" t="n">
-        <v>0.11</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.11</v>
+        <v>0.251</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J7" s="5" t="n">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="K7" s="5" t="n">
-        <v>0.11</v>
+        <v>2.6</v>
       </c>
       <c r="L7" s="5" t="n">
-        <v>0.11</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="C8" s="5" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>0.11</v>
+        <v>0.246</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J8" s="5" t="n">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="K8" s="5" t="n">
-        <v>0.11</v>
+        <v>5.46</v>
       </c>
       <c r="L8" s="5" t="n">
-        <v>0.11</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B9" s="5" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="C9" s="5" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>0.11</v>
+        <v>0.233</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="H9" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I9" s="5" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J9" s="5" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="K9" s="5" t="n">
-        <v>0.11</v>
+        <v>2.75</v>
       </c>
       <c r="L9" s="5" t="n">
-        <v>0.11</v>
+        <v>1.11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B10" s="5" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="C10" s="5" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D10" s="5" t="n">
+        <v>59</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>0.266</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="I10" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="E10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="5" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5" t="n">
-        <v>0</v>
-      </c>
       <c r="J10" s="5" t="n">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="K10" s="5" t="n">
-        <v>0.11</v>
+        <v>3.65</v>
       </c>
       <c r="L10" s="5" t="n">
-        <v>0.11</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B11" s="5" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>0.11</v>
+        <v>0.281</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H11" s="5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I11" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J11" s="5" t="n">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="K11" s="5" t="n">
-        <v>0.11</v>
+        <v>4.53</v>
       </c>
       <c r="L11" s="5" t="n">
-        <v>0.11</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>57</v>
+      </c>
+      <c r="C12" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="D12" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="B12" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="5" t="n">
-        <v>0</v>
-      </c>
       <c r="E12" s="5" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>0.11</v>
+        <v>0.267</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H12" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I12" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J12" s="5" t="n">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="K12" s="5" t="n">
-        <v>0.11</v>
+        <v>3.45</v>
       </c>
       <c r="L12" s="5" t="n">
-        <v>0.11</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B13" s="5" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="C13" s="5" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.11</v>
+        <v>0.249</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I13" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="5" t="n">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="K13" s="5" t="n">
-        <v>0.11</v>
+        <v>3.14</v>
       </c>
       <c r="L13" s="5" t="n">
-        <v>0.11</v>
+        <v>1.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
polishing off new way of running roto but error with change
</commit_message>
<xml_diff>
--- a/src/main/resources/files/stats.xlsx
+++ b/src/main/resources/files/stats.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="52">
   <si>
     <t xml:space="preserve">N</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t xml:space="preserve">Team Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELMATATAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SmokeRunners</t>
   </si>
   <si>
     <t xml:space="preserve">Yeah Jeets!</t>
@@ -391,7 +397,7 @@
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -650,7 +656,7 @@
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2890625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -943,7 +949,7 @@
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1328,7 +1334,7 @@
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1710,10 +1716,10 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="L20" activeCellId="0" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -1764,43 +1770,43 @@
         <v>7</v>
       </c>
       <c r="B2" s="5" t="n">
-        <v>785</v>
+        <v>81</v>
       </c>
       <c r="C2" s="5" t="n">
-        <v>260</v>
+        <v>30</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>741</v>
+        <v>86</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="F2" s="5" t="n">
-        <v>0.236</v>
+        <v>0.267</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>0.752</v>
+        <v>0.829</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="5" t="n">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="J2" s="5" t="n">
-        <v>1606</v>
+        <v>161</v>
       </c>
       <c r="K2" s="5" t="n">
-        <v>3.95</v>
+        <v>4.4</v>
       </c>
       <c r="L2" s="5" t="n">
-        <v>1.22</v>
+        <v>1.37</v>
       </c>
       <c r="M2" s="5" t="n">
-        <v>108</v>
+        <v>9</v>
       </c>
       <c r="N2" s="5" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1808,571 +1814,571 @@
         <v>8</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>708</v>
+        <v>74</v>
       </c>
       <c r="C3" s="5" t="n">
-        <v>208</v>
+        <v>19</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>723</v>
+        <v>76</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.261</v>
+        <v>0.276</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>0.783</v>
+        <v>0.779</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="5" t="n">
-        <v>96</v>
+        <v>13</v>
       </c>
       <c r="J3" s="5" t="n">
-        <v>1386</v>
+        <v>198</v>
       </c>
       <c r="K3" s="5" t="n">
-        <v>4.67</v>
+        <v>4.95</v>
       </c>
       <c r="L3" s="5" t="n">
-        <v>1.37</v>
+        <v>1.41</v>
       </c>
       <c r="M3" s="5" t="n">
-        <v>104</v>
+        <v>10</v>
       </c>
       <c r="N3" s="5" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>737</v>
+        <v>83</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>185</v>
+        <v>16</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>676</v>
+        <v>69</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.269</v>
+        <v>0.257</v>
       </c>
       <c r="G4" s="5" t="n">
-        <v>0.789</v>
+        <v>0.764</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I4" s="5" t="n">
-        <v>91</v>
+        <v>5</v>
       </c>
       <c r="J4" s="5" t="n">
-        <v>1285</v>
+        <v>120</v>
       </c>
       <c r="K4" s="5" t="n">
-        <v>4.04</v>
+        <v>5.89</v>
       </c>
       <c r="L4" s="5" t="n">
-        <v>1.23</v>
+        <v>1.42</v>
       </c>
       <c r="M4" s="5" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="N4" s="5" t="n">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>62</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>83</v>
+      </c>
+      <c r="E5" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="B5" s="5" t="n">
-        <v>751</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>216</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>741</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>74</v>
-      </c>
       <c r="F5" s="5" t="n">
-        <v>0.241</v>
+        <v>0.24</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>0.736</v>
+        <v>0.698</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="I5" s="5" t="n">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="J5" s="5" t="n">
-        <v>1427</v>
+        <v>180</v>
       </c>
       <c r="K5" s="5" t="n">
-        <v>3.78</v>
+        <v>4.54</v>
       </c>
       <c r="L5" s="5" t="n">
-        <v>1.19</v>
+        <v>1.26</v>
       </c>
       <c r="M5" s="5" t="n">
-        <v>109</v>
+        <v>10</v>
       </c>
       <c r="N5" s="5" t="n">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>121</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>98</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>0.296</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>0.883</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="J6" s="5" t="n">
+        <v>166</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <v>4.29</v>
+      </c>
+      <c r="L6" s="5" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="M6" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="B6" s="5" t="n">
-        <v>778</v>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>201</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <v>740</v>
-      </c>
-      <c r="E6" s="5" t="n">
-        <v>115</v>
-      </c>
-      <c r="F6" s="5" t="n">
-        <v>0.259</v>
-      </c>
-      <c r="G6" s="5" t="n">
-        <v>0.769</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="5" t="n">
-        <v>115</v>
-      </c>
-      <c r="J6" s="5" t="n">
-        <v>1559</v>
-      </c>
-      <c r="K6" s="5" t="n">
-        <v>3.55</v>
-      </c>
-      <c r="L6" s="5" t="n">
-        <v>1.17</v>
-      </c>
-      <c r="M6" s="5" t="n">
-        <v>124</v>
-      </c>
       <c r="N6" s="5" t="n">
-        <v>49</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>707</v>
+        <v>66</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>194</v>
+        <v>17</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>713</v>
+        <v>76</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>104</v>
+        <v>18</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.255</v>
+        <v>0.249</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.755</v>
+        <v>0.725</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>87</v>
+        <v>8</v>
       </c>
       <c r="J7" s="5" t="n">
-        <v>1375</v>
+        <v>144</v>
       </c>
       <c r="K7" s="5" t="n">
-        <v>3.84</v>
+        <v>3.97</v>
       </c>
       <c r="L7" s="5" t="n">
-        <v>1.24</v>
+        <v>1.26</v>
       </c>
       <c r="M7" s="5" t="n">
-        <v>107</v>
+        <v>13</v>
       </c>
       <c r="N7" s="5" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>692</v>
+        <v>93</v>
       </c>
       <c r="C8" s="5" t="n">
-        <v>219</v>
+        <v>32</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>688</v>
+        <v>109</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>0.241</v>
+        <v>0.269</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>0.736</v>
+        <v>0.86</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>90</v>
+        <v>4</v>
       </c>
       <c r="J8" s="5" t="n">
-        <v>1503</v>
+        <v>171</v>
       </c>
       <c r="K8" s="5" t="n">
-        <v>3.51</v>
+        <v>4.5</v>
       </c>
       <c r="L8" s="5" t="n">
-        <v>1.16</v>
+        <v>1.34</v>
       </c>
       <c r="M8" s="5" t="n">
-        <v>103</v>
+        <v>8</v>
       </c>
       <c r="N8" s="5" t="n">
-        <v>81</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B9" s="5" t="n">
-        <v>743</v>
+        <v>80</v>
       </c>
       <c r="C9" s="5" t="n">
-        <v>203</v>
+        <v>18</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>749</v>
+        <v>85</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>0.264</v>
+        <v>0.254</v>
       </c>
       <c r="G9" s="5" t="n">
-        <v>0.77</v>
+        <v>0.756</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="I9" s="5" t="n">
-        <v>104</v>
+        <v>13</v>
       </c>
       <c r="J9" s="5" t="n">
-        <v>1500</v>
+        <v>148</v>
       </c>
       <c r="K9" s="5" t="n">
-        <v>3.72</v>
+        <v>4.26</v>
       </c>
       <c r="L9" s="5" t="n">
-        <v>1.24</v>
+        <v>1.44</v>
       </c>
       <c r="M9" s="5" t="n">
-        <v>122</v>
+        <v>10</v>
       </c>
       <c r="N9" s="5" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="5" t="n">
-        <v>700</v>
+        <v>86</v>
       </c>
       <c r="C10" s="5" t="n">
-        <v>199</v>
+        <v>17</v>
       </c>
       <c r="D10" s="5" t="n">
-        <v>731</v>
+        <v>60</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>0.257</v>
+        <v>0.245</v>
       </c>
       <c r="G10" s="5" t="n">
-        <v>0.762</v>
+        <v>0.727</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I10" s="5" t="n">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="J10" s="5" t="n">
-        <v>1299</v>
+        <v>174</v>
       </c>
       <c r="K10" s="5" t="n">
-        <v>3.71</v>
+        <v>4.96</v>
       </c>
       <c r="L10" s="5" t="n">
-        <v>1.21</v>
+        <v>1.37</v>
       </c>
       <c r="M10" s="5" t="n">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="N10" s="5" t="n">
-        <v>95</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B11" s="5" t="n">
-        <v>758</v>
+        <v>77</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>177</v>
+        <v>23</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>697</v>
+        <v>69</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>88</v>
+        <v>6</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>0.258</v>
+        <v>0.25</v>
       </c>
       <c r="G11" s="5" t="n">
-        <v>0.744</v>
+        <v>0.769</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I11" s="5" t="n">
-        <v>96</v>
+        <v>11</v>
       </c>
       <c r="J11" s="5" t="n">
-        <v>1507</v>
+        <v>131</v>
       </c>
       <c r="K11" s="5" t="n">
-        <v>3.55</v>
+        <v>3.86</v>
       </c>
       <c r="L11" s="5" t="n">
-        <v>1.18</v>
+        <v>1.32</v>
       </c>
       <c r="M11" s="5" t="n">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="N11" s="5" t="n">
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5" t="n">
-        <v>715</v>
+        <v>95</v>
       </c>
       <c r="C12" s="5" t="n">
-        <v>214</v>
+        <v>10</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>752</v>
+        <v>59</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>0.248</v>
+        <v>0.297</v>
       </c>
       <c r="G12" s="5" t="n">
-        <v>0.742</v>
+        <v>0.79</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="I12" s="5" t="n">
-        <v>92</v>
+        <v>12</v>
       </c>
       <c r="J12" s="5" t="n">
-        <v>1566</v>
+        <v>190</v>
       </c>
       <c r="K12" s="5" t="n">
-        <v>3.81</v>
+        <v>4.13</v>
       </c>
       <c r="L12" s="5" t="n">
-        <v>1.2</v>
+        <v>1.29</v>
       </c>
       <c r="M12" s="5" t="n">
-        <v>119</v>
+        <v>12</v>
       </c>
       <c r="N12" s="5" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B13" s="5" t="n">
-        <v>795</v>
+        <v>105</v>
       </c>
       <c r="C13" s="5" t="n">
-        <v>216</v>
+        <v>16</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>769</v>
+        <v>81</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.254</v>
+        <v>0.266</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.757</v>
+        <v>0.767</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="I13" s="5" t="n">
-        <v>109</v>
+        <v>10</v>
       </c>
       <c r="J13" s="5" t="n">
-        <v>1556</v>
+        <v>135</v>
       </c>
       <c r="K13" s="5" t="n">
-        <v>3.42</v>
+        <v>4.48</v>
       </c>
       <c r="L13" s="5" t="n">
-        <v>1.16</v>
+        <v>1.43</v>
       </c>
       <c r="M13" s="5" t="n">
-        <v>136</v>
+        <v>9</v>
       </c>
       <c r="N13" s="5" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B14" s="5" t="n">
-        <v>724</v>
+        <v>76</v>
       </c>
       <c r="C14" s="5" t="n">
-        <v>218</v>
+        <v>22</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>750</v>
+        <v>82</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.247</v>
+        <v>0.257</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.74</v>
+        <v>0.741</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="I14" s="5" t="n">
-        <v>103</v>
+        <v>10</v>
       </c>
       <c r="J14" s="5" t="n">
-        <v>1359</v>
+        <v>155</v>
       </c>
       <c r="K14" s="5" t="n">
-        <v>3.91</v>
+        <v>3.93</v>
       </c>
       <c r="L14" s="5" t="n">
-        <v>1.27</v>
+        <v>1.24</v>
       </c>
       <c r="M14" s="5" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="N14" s="5" t="n">
-        <v>31</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="5" t="n">
-        <v>744</v>
+        <v>85</v>
       </c>
       <c r="C15" s="5" t="n">
-        <v>162</v>
+        <v>22</v>
       </c>
       <c r="D15" s="5" t="n">
-        <v>656</v>
+        <v>86</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>126</v>
+        <v>9</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.269</v>
+        <v>0.259</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.751</v>
+        <v>0.762</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I15" s="5" t="n">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="J15" s="5" t="n">
-        <v>1308</v>
+        <v>177</v>
       </c>
       <c r="K15" s="5" t="n">
-        <v>4.16</v>
+        <v>2.63</v>
       </c>
       <c r="L15" s="5" t="n">
-        <v>1.21</v>
+        <v>1.13</v>
       </c>
       <c r="M15" s="5" t="n">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="N15" s="5" t="n">
-        <v>31</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2393,30 +2399,30 @@
     <hyperlink ref="H2" r:id="rId14" display="GOD WILLS IT"/>
     <hyperlink ref="A3" r:id="rId15" display="confusion"/>
     <hyperlink ref="H3" r:id="rId16" display="confusion"/>
-    <hyperlink ref="A4" r:id="rId17" display="DJ's Quality Team"/>
-    <hyperlink ref="H4" r:id="rId18" display="DJ's Quality Team"/>
-    <hyperlink ref="A5" r:id="rId19" display="Epic7"/>
-    <hyperlink ref="H5" r:id="rId20" display="Epic7"/>
-    <hyperlink ref="A6" r:id="rId21" display="Lundo’s Legends"/>
-    <hyperlink ref="H6" r:id="rId22" display="Lundo’s Legends"/>
-    <hyperlink ref="A7" r:id="rId23" display="MillerTime"/>
-    <hyperlink ref="H7" r:id="rId24" display="MillerTime"/>
-    <hyperlink ref="A8" r:id="rId25" display="rainmaker"/>
-    <hyperlink ref="H8" r:id="rId26" display="rainmaker"/>
-    <hyperlink ref="A9" r:id="rId27" display="Samsquanches"/>
-    <hyperlink ref="H9" r:id="rId28" display="Samsquanches"/>
-    <hyperlink ref="A10" r:id="rId29" display="SmokeWalkers"/>
-    <hyperlink ref="H10" r:id="rId30" display="SmokeWalkers"/>
-    <hyperlink ref="A11" r:id="rId31" display="Splitfinger Skadoosh"/>
-    <hyperlink ref="H11" r:id="rId32" display="Splitfinger Skadoosh"/>
-    <hyperlink ref="A12" r:id="rId33" display="Swampnuts"/>
-    <hyperlink ref="H12" r:id="rId34" display="Swampnuts"/>
-    <hyperlink ref="A13" r:id="rId35" display="EL Onće"/>
-    <hyperlink ref="H13" r:id="rId36" display="EL Onće"/>
-    <hyperlink ref="A14" r:id="rId37" display="Mac"/>
-    <hyperlink ref="H14" r:id="rId38" display="Mac"/>
-    <hyperlink ref="A15" r:id="rId39" display="Corbin Copy"/>
-    <hyperlink ref="H15" r:id="rId40" display="Corbin Copy"/>
+    <hyperlink ref="A4" r:id="rId17" display="ELMATATAN"/>
+    <hyperlink ref="H4" r:id="rId18" display="ELMATATAN"/>
+    <hyperlink ref="A5" r:id="rId19" display="SmokeRunners"/>
+    <hyperlink ref="H5" r:id="rId20" display="SmokeRunners"/>
+    <hyperlink ref="A6" r:id="rId21" display="EL Onće"/>
+    <hyperlink ref="H6" r:id="rId22" display="EL Onće"/>
+    <hyperlink ref="A7" r:id="rId23" display="Epic7"/>
+    <hyperlink ref="H7" r:id="rId24" display="Epic7"/>
+    <hyperlink ref="A8" r:id="rId25" display="Lundo’s Legends"/>
+    <hyperlink ref="H8" r:id="rId26" display="Lundo’s Legends"/>
+    <hyperlink ref="A9" r:id="rId27" display="Mac"/>
+    <hyperlink ref="H9" r:id="rId28" display="Mac"/>
+    <hyperlink ref="A10" r:id="rId29" display="MillerTime"/>
+    <hyperlink ref="H10" r:id="rId30" display="MillerTime"/>
+    <hyperlink ref="A11" r:id="rId31" display="rainmaker"/>
+    <hyperlink ref="H11" r:id="rId32" display="rainmaker"/>
+    <hyperlink ref="A12" r:id="rId33" display="Samsquanches"/>
+    <hyperlink ref="H12" r:id="rId34" display="Samsquanches"/>
+    <hyperlink ref="A13" r:id="rId35" display="SmokeWalkers"/>
+    <hyperlink ref="H13" r:id="rId36" display="SmokeWalkers"/>
+    <hyperlink ref="A14" r:id="rId37" display="Splitfinger Skadoosh"/>
+    <hyperlink ref="H14" r:id="rId38" display="Splitfinger Skadoosh"/>
+    <hyperlink ref="A15" r:id="rId39" display="Swampnuts"/>
+    <hyperlink ref="H15" r:id="rId40" display="Swampnuts"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2439,7 +2445,7 @@
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -2481,230 +2487,230 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>65</v>
+        <v>114</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0.828</v>
+        <v>0.819</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>87</v>
+        <v>142</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>2.74</v>
+        <v>3.16</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>1.16</v>
+        <v>1.27</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0.819</v>
+        <v>0.839</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>136</v>
+        <v>219</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>3.11</v>
+        <v>3.44</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>1.19</v>
+        <v>1.26</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>112</v>
+      </c>
+      <c r="C4" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>81</v>
-      </c>
-      <c r="C4" s="2" t="n">
+      <c r="D4" s="2" t="n">
+        <v>114</v>
+      </c>
+      <c r="E4" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="D4" s="2" t="n">
-        <v>74</v>
-      </c>
-      <c r="E4" s="2" t="n">
+      <c r="F4" s="2" t="n">
+        <v>0.833</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>171</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="K4" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="F4" s="2" t="n">
-        <v>0.906</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>106</v>
-      </c>
-      <c r="I4" s="2" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="J4" s="2" t="n">
-        <v>1.47</v>
-      </c>
-      <c r="K4" s="2" t="n">
-        <v>5</v>
-      </c>
       <c r="L4" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.743</v>
+        <v>0.712</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>93</v>
+        <v>178</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>2.52</v>
+        <v>4.14</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>1.04</v>
+        <v>1.18</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0.77</v>
+        <v>0.768</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>120</v>
+        <v>208</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>5.1</v>
+        <v>4.87</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>1.27</v>
+        <v>1.32</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>0.72</v>
+        <v>0.807</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>142</v>
+        <v>231</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>4.84</v>
+        <v>4.02</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>1.38</v>
+        <v>1.27</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2712,151 +2718,151 @@
         <v>9</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>0.855</v>
+        <v>0.793</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>105</v>
+        <v>163</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>4.25</v>
+        <v>4.14</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>1.37</v>
+        <v>1.34</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>65</v>
+        <v>117</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>66</v>
+        <v>119</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>0.828</v>
+        <v>0.805</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>100</v>
+        <v>189</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>5.02</v>
+        <v>4.7</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>1.47</v>
+        <v>1.37</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>59</v>
+        <v>106</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="E10" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>182</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>4.28</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="K10" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="F10" s="2" t="n">
-        <v>0.723</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>109</v>
-      </c>
-      <c r="I10" s="2" t="n">
-        <v>5.15</v>
-      </c>
-      <c r="J10" s="2" t="n">
-        <v>1.31</v>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>6</v>
-      </c>
       <c r="L10" s="2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0.787</v>
+        <v>0.741</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>95</v>
+        <v>170</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>3.98</v>
+        <v>4.31</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>1.42</v>
+        <v>1.43</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2903,7 +2909,7 @@
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -2931,7 +2937,7 @@
         <v>22</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>17</v>
@@ -2945,7 +2951,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>62</v>
@@ -2963,7 +2969,7 @@
         <v>0.305</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H2" s="5" t="n">
         <v>8</v>
@@ -2983,7 +2989,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B3" s="5" t="n">
         <v>59</v>
@@ -3001,7 +3007,7 @@
         <v>0.288</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H3" s="5" t="n">
         <v>7</v>
@@ -3021,7 +3027,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B4" s="5" t="n">
         <v>55</v>
@@ -3039,7 +3045,7 @@
         <v>0.294</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H4" s="5" t="n">
         <v>3</v>
@@ -3059,7 +3065,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B5" s="5" t="n">
         <v>57</v>
@@ -3077,7 +3083,7 @@
         <v>0.241</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H5" s="5" t="n">
         <v>4</v>
@@ -3097,7 +3103,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B6" s="5" t="n">
         <v>49</v>
@@ -3115,7 +3121,7 @@
         <v>0.271</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H6" s="5" t="n">
         <v>7</v>
@@ -3135,7 +3141,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" s="5" t="n">
         <v>41</v>
@@ -3153,7 +3159,7 @@
         <v>0.251</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H7" s="5" t="n">
         <v>3</v>
@@ -3173,7 +3179,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>56</v>
@@ -3191,7 +3197,7 @@
         <v>0.246</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H8" s="5" t="n">
         <v>4</v>
@@ -3211,7 +3217,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B9" s="5" t="n">
         <v>48</v>
@@ -3229,7 +3235,7 @@
         <v>0.233</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H9" s="5" t="n">
         <v>5</v>
@@ -3249,7 +3255,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>57</v>
@@ -3267,7 +3273,7 @@
         <v>0.266</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H10" s="5" t="n">
         <v>6</v>
@@ -3287,7 +3293,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B11" s="5" t="n">
         <v>54</v>
@@ -3305,7 +3311,7 @@
         <v>0.281</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H11" s="5" t="n">
         <v>4</v>
@@ -3325,7 +3331,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>57</v>
@@ -3343,7 +3349,7 @@
         <v>0.267</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H12" s="5" t="n">
         <v>5</v>
@@ -3363,7 +3369,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B13" s="5" t="n">
         <v>43</v>
@@ -3381,7 +3387,7 @@
         <v>0.249</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H13" s="5" t="n">
         <v>9</v>

</xml_diff>

<commit_message>
small changes as I smooth over runner for all or one league
</commit_message>
<xml_diff>
--- a/src/main/resources/files/stats.xlsx
+++ b/src/main/resources/files/stats.xlsx
@@ -115,7 +115,7 @@
     <t xml:space="preserve">ELMATATAN</t>
   </si>
   <si>
-    <t xml:space="preserve">SmokeRunners</t>
+    <t xml:space="preserve">snowmaker</t>
   </si>
   <si>
     <t xml:space="preserve">Yeah Jeets!</t>
@@ -397,7 +397,7 @@
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -656,7 +656,7 @@
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2890625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.30078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -949,7 +949,7 @@
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1334,7 +1334,7 @@
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1713,13 +1713,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L20" activeCellId="0" sqref="L20"/>
+      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -1770,40 +1770,40 @@
         <v>7</v>
       </c>
       <c r="B2" s="5" t="n">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="C2" s="5" t="n">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>86</v>
+        <v>117</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F2" s="5" t="n">
-        <v>0.267</v>
+        <v>0.25</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>0.829</v>
+        <v>0.77</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="5" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J2" s="5" t="n">
-        <v>161</v>
+        <v>239</v>
       </c>
       <c r="K2" s="5" t="n">
-        <v>4.4</v>
+        <v>4.22</v>
       </c>
       <c r="L2" s="5" t="n">
-        <v>1.37</v>
+        <v>1.29</v>
       </c>
       <c r="M2" s="5" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="N2" s="5" t="n">
         <v>0</v>
@@ -1814,43 +1814,43 @@
         <v>8</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="C3" s="5" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.276</v>
+        <v>0.271</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>0.779</v>
+        <v>0.788</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="5" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="J3" s="5" t="n">
-        <v>198</v>
+        <v>256</v>
       </c>
       <c r="K3" s="5" t="n">
-        <v>4.95</v>
+        <v>4.83</v>
       </c>
       <c r="L3" s="5" t="n">
-        <v>1.41</v>
+        <v>1.4</v>
       </c>
       <c r="M3" s="5" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N3" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1858,43 +1858,43 @@
         <v>28</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.257</v>
+        <v>0.258</v>
       </c>
       <c r="G4" s="5" t="n">
-        <v>0.764</v>
+        <v>0.762</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>28</v>
       </c>
       <c r="I4" s="5" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J4" s="5" t="n">
-        <v>120</v>
+        <v>172</v>
       </c>
       <c r="K4" s="5" t="n">
-        <v>5.89</v>
+        <v>5.48</v>
       </c>
       <c r="L4" s="5" t="n">
-        <v>1.42</v>
+        <v>1.33</v>
       </c>
       <c r="M4" s="5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N4" s="5" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1902,43 +1902,43 @@
         <v>29</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>62</v>
+        <v>103</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>0.24</v>
+        <v>0.258</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>0.698</v>
+        <v>0.757</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>29</v>
       </c>
       <c r="I5" s="5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J5" s="5" t="n">
-        <v>180</v>
+        <v>221</v>
       </c>
       <c r="K5" s="5" t="n">
-        <v>4.54</v>
+        <v>4.07</v>
       </c>
       <c r="L5" s="5" t="n">
-        <v>1.26</v>
+        <v>1.2</v>
       </c>
       <c r="M5" s="5" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N5" s="5" t="n">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1946,40 +1946,40 @@
         <v>24</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>121</v>
+        <v>174</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>98</v>
+        <v>155</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>0.296</v>
+        <v>0.292</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>0.883</v>
+        <v>0.904</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I6" s="5" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J6" s="5" t="n">
-        <v>166</v>
+        <v>236</v>
       </c>
       <c r="K6" s="5" t="n">
-        <v>4.29</v>
+        <v>4.32</v>
       </c>
       <c r="L6" s="5" t="n">
-        <v>1.35</v>
+        <v>1.34</v>
       </c>
       <c r="M6" s="5" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="N6" s="5" t="n">
         <v>2</v>
@@ -1990,43 +1990,43 @@
         <v>9</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="E7" s="5" t="n">
         <v>18</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.249</v>
+        <v>0.237</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.725</v>
+        <v>0.702</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J7" s="5" t="n">
-        <v>144</v>
+        <v>208</v>
       </c>
       <c r="K7" s="5" t="n">
-        <v>3.97</v>
+        <v>3.81</v>
       </c>
       <c r="L7" s="5" t="n">
-        <v>1.26</v>
+        <v>1.18</v>
       </c>
       <c r="M7" s="5" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N7" s="5" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2034,40 +2034,40 @@
         <v>12</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="C8" s="5" t="n">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>109</v>
+        <v>148</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>0.269</v>
+        <v>0.262</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>0.86</v>
+        <v>0.836</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J8" s="5" t="n">
-        <v>171</v>
+        <v>252</v>
       </c>
       <c r="K8" s="5" t="n">
-        <v>4.5</v>
+        <v>4.43</v>
       </c>
       <c r="L8" s="5" t="n">
-        <v>1.34</v>
+        <v>1.3</v>
       </c>
       <c r="M8" s="5" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="N8" s="5" t="n">
         <v>1</v>
@@ -2078,43 +2078,43 @@
         <v>23</v>
       </c>
       <c r="B9" s="5" t="n">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="C9" s="5" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>0.254</v>
+        <v>0.258</v>
       </c>
       <c r="G9" s="5" t="n">
-        <v>0.756</v>
+        <v>0.77</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="5" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J9" s="5" t="n">
-        <v>148</v>
+        <v>217</v>
       </c>
       <c r="K9" s="5" t="n">
-        <v>4.26</v>
+        <v>3.88</v>
       </c>
       <c r="L9" s="5" t="n">
-        <v>1.44</v>
+        <v>1.29</v>
       </c>
       <c r="M9" s="5" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="N9" s="5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2122,43 +2122,43 @@
         <v>14</v>
       </c>
       <c r="B10" s="5" t="n">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="C10" s="5" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D10" s="5" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>0.245</v>
+        <v>0.246</v>
       </c>
       <c r="G10" s="5" t="n">
-        <v>0.727</v>
+        <v>0.724</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I10" s="5" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J10" s="5" t="n">
-        <v>174</v>
+        <v>241</v>
       </c>
       <c r="K10" s="5" t="n">
-        <v>4.96</v>
+        <v>4.97</v>
       </c>
       <c r="L10" s="5" t="n">
         <v>1.37</v>
       </c>
       <c r="M10" s="5" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="N10" s="5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2166,43 +2166,43 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="n">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="C11" s="5" t="n">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>0.25</v>
+        <v>0.238</v>
       </c>
       <c r="G11" s="5" t="n">
-        <v>0.769</v>
+        <v>0.723</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="I11" s="5" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="J11" s="5" t="n">
-        <v>131</v>
+        <v>188</v>
       </c>
       <c r="K11" s="5" t="n">
-        <v>3.86</v>
+        <v>4.25</v>
       </c>
       <c r="L11" s="5" t="n">
-        <v>1.32</v>
+        <v>1.31</v>
       </c>
       <c r="M11" s="5" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N11" s="5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2210,43 +2210,43 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="n">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="C12" s="5" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>0.297</v>
+        <v>0.287</v>
       </c>
       <c r="G12" s="5" t="n">
-        <v>0.79</v>
+        <v>0.789</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="5" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="J12" s="5" t="n">
-        <v>190</v>
+        <v>260</v>
       </c>
       <c r="K12" s="5" t="n">
-        <v>4.13</v>
+        <v>3.91</v>
       </c>
       <c r="L12" s="5" t="n">
-        <v>1.29</v>
+        <v>1.25</v>
       </c>
       <c r="M12" s="5" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="N12" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2254,43 +2254,43 @@
         <v>13</v>
       </c>
       <c r="B13" s="5" t="n">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="C13" s="5" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>0.266</v>
+        <v>0.274</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>0.767</v>
+        <v>0.789</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="I13" s="5" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J13" s="5" t="n">
-        <v>135</v>
+        <v>215</v>
       </c>
       <c r="K13" s="5" t="n">
-        <v>4.48</v>
+        <v>4.14</v>
       </c>
       <c r="L13" s="5" t="n">
-        <v>1.43</v>
+        <v>1.32</v>
       </c>
       <c r="M13" s="5" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="N13" s="5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2298,43 +2298,43 @@
         <v>16</v>
       </c>
       <c r="B14" s="5" t="n">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="C14" s="5" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>82</v>
+        <v>116</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>0.257</v>
+        <v>0.25</v>
       </c>
       <c r="G14" s="5" t="n">
-        <v>0.741</v>
+        <v>0.728</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>16</v>
       </c>
       <c r="I14" s="5" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J14" s="5" t="n">
-        <v>155</v>
+        <v>224</v>
       </c>
       <c r="K14" s="5" t="n">
-        <v>3.93</v>
+        <v>4.12</v>
       </c>
       <c r="L14" s="5" t="n">
-        <v>1.24</v>
+        <v>1.28</v>
       </c>
       <c r="M14" s="5" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N14" s="5" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2342,45 +2342,46 @@
         <v>25</v>
       </c>
       <c r="B15" s="5" t="n">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="C15" s="5" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D15" s="5" t="n">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F15" s="5" t="n">
-        <v>0.259</v>
+        <v>0.249</v>
       </c>
       <c r="G15" s="5" t="n">
-        <v>0.762</v>
+        <v>0.724</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>25</v>
       </c>
       <c r="I15" s="5" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="J15" s="5" t="n">
-        <v>177</v>
+        <v>221</v>
       </c>
       <c r="K15" s="5" t="n">
-        <v>2.63</v>
+        <v>2.83</v>
       </c>
       <c r="L15" s="5" t="n">
-        <v>1.13</v>
+        <v>1.16</v>
       </c>
       <c r="M15" s="5" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="N15" s="5" t="n">
         <v>7</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="R"/>
@@ -2401,8 +2402,8 @@
     <hyperlink ref="H3" r:id="rId16" display="confusion"/>
     <hyperlink ref="A4" r:id="rId17" display="ELMATATAN"/>
     <hyperlink ref="H4" r:id="rId18" display="ELMATATAN"/>
-    <hyperlink ref="A5" r:id="rId19" display="SmokeRunners"/>
-    <hyperlink ref="H5" r:id="rId20" display="SmokeRunners"/>
+    <hyperlink ref="A5" r:id="rId19" display="snowmaker"/>
+    <hyperlink ref="H5" r:id="rId20" display="snowmaker"/>
     <hyperlink ref="A6" r:id="rId21" display="EL Onće"/>
     <hyperlink ref="H6" r:id="rId22" display="EL Onće"/>
     <hyperlink ref="A7" r:id="rId23" display="Epic7"/>
@@ -2442,46 +2443,46 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2489,37 +2490,37 @@
       <c r="A2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>112</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>35</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>114</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>0.819</v>
+      <c r="B2" s="5" t="n">
+        <v>149</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>140</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>0.769</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="2" t="n">
-        <v>142</v>
-      </c>
-      <c r="I2" s="2" t="n">
-        <v>3.16</v>
-      </c>
-      <c r="J2" s="2" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="K2" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="L2" s="2" t="n">
+      <c r="H2" s="5" t="n">
+        <v>215</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="J2" s="5" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="K2" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="L2" s="5" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2527,113 +2528,113 @@
       <c r="A3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>98</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>105</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>14</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>0.839</v>
+      <c r="B3" s="5" t="n">
+        <v>130</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>43</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>138</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>0.822</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="2" t="n">
-        <v>219</v>
-      </c>
-      <c r="I3" s="2" t="n">
-        <v>3.44</v>
-      </c>
-      <c r="J3" s="2" t="n">
-        <v>1.26</v>
-      </c>
-      <c r="K3" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="L3" s="2" t="n">
-        <v>8</v>
+      <c r="H3" s="5" t="n">
+        <v>290</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="J3" s="5" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="K3" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="L3" s="5" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>112</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>114</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>19</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>0.833</v>
+      <c r="B4" s="5" t="n">
+        <v>156</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>45</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>160</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0.819</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="2" t="n">
-        <v>171</v>
-      </c>
-      <c r="I4" s="2" t="n">
-        <v>3.78</v>
-      </c>
-      <c r="J4" s="2" t="n">
+      <c r="H4" s="5" t="n">
+        <v>241</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="J4" s="5" t="n">
         <v>1.4</v>
       </c>
-      <c r="K4" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="L4" s="2" t="n">
-        <v>3</v>
+      <c r="K4" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="L4" s="5" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="2" t="n">
-        <v>103</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>92</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>17</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>0.712</v>
+      <c r="B5" s="5" t="n">
+        <v>150</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>134</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>24</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0.745</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="2" t="n">
-        <v>178</v>
-      </c>
-      <c r="I5" s="2" t="n">
-        <v>4.14</v>
-      </c>
-      <c r="J5" s="2" t="n">
-        <v>1.18</v>
-      </c>
-      <c r="K5" s="2" t="n">
-        <v>14</v>
-      </c>
-      <c r="L5" s="2" t="n">
+      <c r="H5" s="5" t="n">
+        <v>252</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <v>4.59</v>
+      </c>
+      <c r="J5" s="5" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="K5" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="L5" s="5" t="n">
         <v>3</v>
       </c>
     </row>
@@ -2641,252 +2642,262 @@
       <c r="A6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="2" t="n">
-        <v>91</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>93</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>0.768</v>
+      <c r="B6" s="5" t="n">
+        <v>129</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>138</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>0.776</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="2" t="n">
-        <v>208</v>
-      </c>
-      <c r="I6" s="2" t="n">
-        <v>4.87</v>
-      </c>
-      <c r="J6" s="2" t="n">
-        <v>1.32</v>
-      </c>
-      <c r="K6" s="2" t="n">
-        <v>13</v>
-      </c>
-      <c r="L6" s="2" t="n">
-        <v>-1</v>
+      <c r="H6" s="5" t="n">
+        <v>278</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>4.67</v>
+      </c>
+      <c r="J6" s="5" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="L6" s="5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="2" t="n">
-        <v>101</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>93</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>23</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>0.807</v>
+      <c r="B7" s="5" t="n">
+        <v>141</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>41</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>118</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>0.816</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="2" t="n">
-        <v>231</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <v>4.02</v>
-      </c>
-      <c r="J7" s="2" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="K7" s="2" t="n">
-        <v>15</v>
-      </c>
-      <c r="L7" s="2" t="n">
-        <v>7</v>
+      <c r="H7" s="5" t="n">
+        <v>351</v>
+      </c>
+      <c r="I7" s="5" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="J7" s="5" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="K7" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="L7" s="5" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2" t="n">
-        <v>115</v>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>26</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>87</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="F8" s="2" t="n">
-        <v>0.793</v>
+      <c r="B8" s="5" t="n">
+        <v>147</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>111</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>0.759</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="2" t="n">
-        <v>163</v>
-      </c>
-      <c r="I8" s="2" t="n">
-        <v>4.14</v>
-      </c>
-      <c r="J8" s="2" t="n">
-        <v>1.34</v>
-      </c>
-      <c r="K8" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="L8" s="2" t="n">
-        <v>7</v>
+      <c r="H8" s="5" t="n">
+        <v>230</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="J8" s="5" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="K8" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="L8" s="5" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="2" t="n">
-        <v>117</v>
-      </c>
-      <c r="C9" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>119</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="F9" s="2" t="n">
-        <v>0.805</v>
+      <c r="B9" s="5" t="n">
+        <v>172</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>41</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>170</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>0.801</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="2" t="n">
-        <v>189</v>
-      </c>
-      <c r="I9" s="2" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="J9" s="2" t="n">
-        <v>1.37</v>
-      </c>
-      <c r="K9" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="L9" s="2" t="n">
-        <v>4</v>
+      <c r="H9" s="5" t="n">
+        <v>293</v>
+      </c>
+      <c r="I9" s="5" t="n">
+        <v>4.64</v>
+      </c>
+      <c r="J9" s="5" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="K9" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="L9" s="5" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="2" t="n">
-        <v>106</v>
-      </c>
-      <c r="C10" s="2" t="n">
-        <v>26</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>105</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>19</v>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>0.77</v>
+      <c r="B10" s="5" t="n">
+        <v>153</v>
+      </c>
+      <c r="C10" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>151</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>0.78</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="2" t="n">
-        <v>182</v>
-      </c>
-      <c r="I10" s="2" t="n">
-        <v>4.28</v>
-      </c>
-      <c r="J10" s="2" t="n">
-        <v>1.26</v>
-      </c>
-      <c r="K10" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="L10" s="2" t="n">
-        <v>10</v>
+      <c r="H10" s="5" t="n">
+        <v>237</v>
+      </c>
+      <c r="I10" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="J10" s="5" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="K10" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="L10" s="5" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="2" t="n">
-        <v>97</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>92</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>29</v>
-      </c>
-      <c r="F11" s="2" t="n">
-        <v>0.741</v>
+      <c r="B11" s="5" t="n">
+        <v>132</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>131</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>0.736</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="2" t="n">
-        <v>170</v>
-      </c>
-      <c r="I11" s="2" t="n">
-        <v>4.31</v>
-      </c>
-      <c r="J11" s="2" t="n">
-        <v>1.43</v>
-      </c>
-      <c r="K11" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="L11" s="2" t="n">
-        <v>5</v>
+      <c r="H11" s="5" t="n">
+        <v>228</v>
+      </c>
+      <c r="I11" s="5" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="J11" s="5" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="K11" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="L11" s="5" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="Yeah Jeets!"/>
-    <hyperlink ref="G2" r:id="rId2" display="Yeah Jeets!"/>
-    <hyperlink ref="A3" r:id="rId3" display="raincrafter"/>
-    <hyperlink ref="G3" r:id="rId4" display="raincrafter"/>
-    <hyperlink ref="A4" r:id="rId5" display="Cue the Duckboats"/>
-    <hyperlink ref="G4" r:id="rId6" display="Cue the Duckboats"/>
-    <hyperlink ref="A5" r:id="rId7" display="Smokescreen"/>
-    <hyperlink ref="G5" r:id="rId8" display="Smokescreen"/>
-    <hyperlink ref="A6" r:id="rId9" display="ShohTime"/>
-    <hyperlink ref="G6" r:id="rId10" display="ShohTime"/>
-    <hyperlink ref="A7" r:id="rId11" display="RobbNen#31"/>
-    <hyperlink ref="G7" r:id="rId12" display="RobbNen#31"/>
-    <hyperlink ref="A8" r:id="rId13" display="Epic7"/>
-    <hyperlink ref="G8" r:id="rId14" display="Epic7"/>
-    <hyperlink ref="A9" r:id="rId15" display="Leandres"/>
-    <hyperlink ref="G9" r:id="rId16" display="Leandres"/>
-    <hyperlink ref="A10" r:id="rId17" display="Joe's Nice Team"/>
-    <hyperlink ref="G10" r:id="rId18" display="Joe's Nice Team"/>
-    <hyperlink ref="A11" r:id="rId19" display="Matt's Marvelous Team"/>
-    <hyperlink ref="G11" r:id="rId20" display="Matt's Marvelous Team"/>
+    <hyperlink ref="B1" r:id="rId1" display="R"/>
+    <hyperlink ref="C1" r:id="rId2" display="HR"/>
+    <hyperlink ref="D1" r:id="rId3" display="RBI"/>
+    <hyperlink ref="E1" r:id="rId4" display="SB"/>
+    <hyperlink ref="F1" r:id="rId5" display="OPS"/>
+    <hyperlink ref="H1" r:id="rId6" display="K"/>
+    <hyperlink ref="I1" r:id="rId7" display="ERA"/>
+    <hyperlink ref="J1" r:id="rId8" display="WHIP"/>
+    <hyperlink ref="K1" r:id="rId9" display="QS"/>
+    <hyperlink ref="L1" r:id="rId10" display="NSV"/>
+    <hyperlink ref="A2" r:id="rId11" display="Yeah Jeets!"/>
+    <hyperlink ref="G2" r:id="rId12" display="Yeah Jeets!"/>
+    <hyperlink ref="A3" r:id="rId13" display="raincrafter"/>
+    <hyperlink ref="G3" r:id="rId14" display="raincrafter"/>
+    <hyperlink ref="A4" r:id="rId15" display="Cue the Duckboats"/>
+    <hyperlink ref="G4" r:id="rId16" display="Cue the Duckboats"/>
+    <hyperlink ref="A5" r:id="rId17" display="Smokescreen"/>
+    <hyperlink ref="G5" r:id="rId18" display="Smokescreen"/>
+    <hyperlink ref="A6" r:id="rId19" display="ShohTime"/>
+    <hyperlink ref="G6" r:id="rId20" display="ShohTime"/>
+    <hyperlink ref="A7" r:id="rId21" display="RobbNen#31"/>
+    <hyperlink ref="G7" r:id="rId22" display="RobbNen#31"/>
+    <hyperlink ref="A8" r:id="rId23" display="Epic7"/>
+    <hyperlink ref="G8" r:id="rId24" display="Epic7"/>
+    <hyperlink ref="A9" r:id="rId25" display="Leandres"/>
+    <hyperlink ref="G9" r:id="rId26" display="Leandres"/>
+    <hyperlink ref="A10" r:id="rId27" display="Joe's Nice Team"/>
+    <hyperlink ref="G10" r:id="rId28" display="Joe's Nice Team"/>
+    <hyperlink ref="A11" r:id="rId29" display="Matt's Marvelous Team"/>
+    <hyperlink ref="G11" r:id="rId30" display="Matt's Marvelous Team"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2909,7 +2920,7 @@
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">

</xml_diff>